<commit_message>
get no of columns in excel sheet
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelSheet/Recruitment.xlsx
+++ b/src/test/resources/ExcelSheet/Recruitment.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\OrangeHRMintel\data-driven-test-automation\src\test\resources\ExcelSheet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Anushanth\Test Automation\src\test\resources\ExcelSheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31C489A8-3769-4B15-B2CB-F2D63EE1AB50}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97989ABF-48E5-43D0-B15B-FEFDE7D85B64}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="1230" windowWidth="9585" windowHeight="7875" xr2:uid="{E29C7E7B-C0AD-4B25-964C-1D6B60FEA2E2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{E29C7E7B-C0AD-4B25-964C-1D6B60FEA2E2}"/>
   </bookViews>
   <sheets>
     <sheet name="AddVacancy" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="37">
   <si>
     <t>JobTitle</t>
   </si>
@@ -131,7 +131,13 @@
     <t>very soon</t>
   </si>
   <si>
-    <t>accounts</t>
+    <t>test1</t>
+  </si>
+  <si>
+    <t>test2</t>
+  </si>
+  <si>
+    <t>test3</t>
   </si>
 </sst>
 </file>
@@ -514,10 +520,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9087A582-C57A-4FC5-8718-FA54721B73FC}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -560,6 +566,40 @@
         <v>3</v>
       </c>
       <c r="E2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add recruitment candidate details
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelSheet/Recruitment.xlsx
+++ b/src/test/resources/ExcelSheet/Recruitment.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\OrangeHRMintel\data-driven-test-automation\src\test\resources\ExcelSheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31C489A8-3769-4B15-B2CB-F2D63EE1AB50}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BD4C38B-0B95-4A22-ABE8-467389E7CA50}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="1230" windowWidth="9585" windowHeight="7875" xr2:uid="{E29C7E7B-C0AD-4B25-964C-1D6B60FEA2E2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{E29C7E7B-C0AD-4B25-964C-1D6B60FEA2E2}"/>
   </bookViews>
   <sheets>
     <sheet name="AddVacancy" sheetId="1" r:id="rId1"/>
@@ -516,7 +516,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9087A582-C57A-4FC5-8718-FA54721B73FC}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -573,8 +573,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94C98F44-D38A-4170-8007-DA6BF683D58D}">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
login test & report generation & screenshot
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelSheet/Recruitment.xlsx
+++ b/src/test/resources/ExcelSheet/Recruitment.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\OrangeHRMintel\data-driven-test-automation\src\test\resources\ExcelSheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2E2E279-47F4-4306-8C02-E6F624AE4EB0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15C96F54-440A-40F3-932C-238DE4A71CA5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{E29C7E7B-C0AD-4B25-964C-1D6B60FEA2E2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="846" activeTab="5" xr2:uid="{E29C7E7B-C0AD-4B25-964C-1D6B60FEA2E2}"/>
   </bookViews>
   <sheets>
     <sheet name="AddCandidate" sheetId="3" r:id="rId1"/>
     <sheet name="EditVacancy" sheetId="5" r:id="rId2"/>
     <sheet name="EditCandidate" sheetId="6" r:id="rId3"/>
-    <sheet name="SearchVacancy" sheetId="4" r:id="rId4"/>
-    <sheet name="AddVacancy" sheetId="1" r:id="rId5"/>
-    <sheet name="SearchCandidate" sheetId="2" r:id="rId6"/>
+    <sheet name="Login" sheetId="7" r:id="rId4"/>
+    <sheet name="SearchVacancy" sheetId="4" r:id="rId5"/>
+    <sheet name="AddVacancy" sheetId="1" r:id="rId6"/>
+    <sheet name="SearchCandidate" sheetId="2" r:id="rId7"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="55">
   <si>
     <t>JobTitle</t>
   </si>
@@ -156,6 +157,45 @@
   </si>
   <si>
     <t>Quality Engineer</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>admin123</t>
+  </si>
+  <si>
+    <t>ghh</t>
+  </si>
+  <si>
+    <t>ddd</t>
+  </si>
+  <si>
+    <t>login success</t>
+  </si>
+  <si>
+    <t>valid</t>
+  </si>
+  <si>
+    <t>invalid</t>
+  </si>
+  <si>
+    <t>alertmsg</t>
+  </si>
+  <si>
+    <t>Invalid credentials</t>
+  </si>
+  <si>
+    <t>Username cannot be empty</t>
+  </si>
+  <si>
+    <t>Password cannot be empty</t>
   </si>
 </sst>
 </file>
@@ -694,7 +734,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E848881E-3EBE-4F22-8597-2FB72BE73A6E}">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
@@ -704,6 +744,7 @@
     <col min="5" max="5" width="18.5703125" customWidth="1"/>
     <col min="6" max="6" width="15.7109375" customWidth="1"/>
     <col min="8" max="8" width="15.7109375" customWidth="1"/>
+    <col min="9" max="9" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -773,6 +814,128 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF5EBF32-6A0D-4364-95BC-DE630C705D0E}">
+  <dimension ref="A1:D8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" customWidth="1"/>
+    <col min="4" max="4" width="29.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>878</v>
+      </c>
+      <c r="C6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FE3DFDE-B504-40E6-B1CF-A98834D271D5}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -821,12 +984,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9087A582-C57A-4FC5-8718-FA54721B73FC}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -866,7 +1029,7 @@
         <v>7</v>
       </c>
       <c r="D2">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E2" t="s">
         <v>5</v>
@@ -878,7 +1041,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AAC20FD-30FB-40DF-A8F2-108AD3421608}">
   <dimension ref="A1:I2"/>
   <sheetViews>

</xml_diff>

<commit_message>
recruitment,time test regression modify
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelSheet/Recruitment.xlsx
+++ b/src/test/resources/ExcelSheet/Recruitment.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\OrangeHRMintel\data-driven-test-automation\src\test\resources\ExcelSheet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\invictaAutomation\data-driven-test-automation\src\test\resources\ExcelSheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15C96F54-440A-40F3-932C-238DE4A71CA5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{874D23D4-B94E-4C6E-AEB7-C41474AD219F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="846" activeTab="5" xr2:uid="{E29C7E7B-C0AD-4B25-964C-1D6B60FEA2E2}"/>
+    <workbookView xWindow="390" yWindow="1230" windowWidth="9585" windowHeight="7875" tabRatio="846" activeTab="5" xr2:uid="{E29C7E7B-C0AD-4B25-964C-1D6B60FEA2E2}"/>
   </bookViews>
   <sheets>
     <sheet name="AddCandidate" sheetId="3" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="56">
   <si>
     <t>JobTitle</t>
   </si>
@@ -196,6 +196,9 @@
   </si>
   <si>
     <t>Password cannot be empty</t>
+  </si>
+  <si>
+    <t>Russel Hamilton</t>
   </si>
 </sst>
 </file>
@@ -989,7 +992,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1026,7 +1029,7 @@
         <v>33</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>55</v>
       </c>
       <c r="D2">
         <v>6</v>

</xml_diff>